<commit_message>
Concept Maps immunization e Allergy
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Alergias/ConceptMapsAlergia/bralergenoscbara-sct.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Alergias/ConceptMapsAlergia/bralergenoscbara-sct.xlsx
@@ -8,21 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/1.RepositorioSemantico/Alergias/ConceptMapsAlergia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9F6099-D724-D046-B6E8-6DC4EB061302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB313EFA-3F09-0D46-9C31-CDE2314D8820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Equivalências" sheetId="2" r:id="rId1"/>
-    <sheet name="alergenos-cbara" sheetId="1" r:id="rId2"/>
-    <sheet name="Totais" sheetId="3" r:id="rId3"/>
+    <sheet name="alergenos-cbara" sheetId="1" r:id="rId1"/>
+    <sheet name="Totais" sheetId="3" r:id="rId2"/>
+    <sheet name="Equivalências" sheetId="2" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'alergenos-cbara'!$B$3:$J$155</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="1">'alergenos-cbara'!$I$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'alergenos-cbara'!$B$3:$J$155</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">'alergenos-cbara'!$I$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1642,19 +1639,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Opções"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1919,49 +1903,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E25" sqref="E25:G145"/>
     </sheetView>
   </sheetViews>
@@ -6079,27 +6025,22 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:L155">
     <sortCondition ref="C4:C155"/>
   </sortState>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"1..1,1..*,*..1,*..*"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Equivalências!$A$1:$G$1</xm:f>
           </x14:formula1>
           <xm:sqref>I4:I1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>'/Users/beatrizdefarialeao/Library/Containers/com.microsoft.Excel/Data/Documents/Users\beatrizdefarialeao\Library\Containers\com.microsoft.Excel\Data\Documents\C:\Users\moaassis\Documents\HSL-IPS\Entregaveis\Mapeamentos\Templates\ConceptMap\BRImunobiológico\[Mapping BRImunobiológico.xlsx]Opções'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>I3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6107,11 +6048,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5ECD1F8-2B9D-C347-9AC8-762B8811C9BC}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:D8"/>
     </sheetView>
   </sheetViews>
@@ -6210,4 +6151,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>